<commit_message>
finished affirm, going to atarc
</commit_message>
<xml_diff>
--- a/fed-events/Fed_Events-03.25.23.xlsx
+++ b/fed-events/Fed_Events-03.25.23.xlsx
@@ -12,13 +12,14 @@
     <sheet name="Nextgov" sheetId="3" r:id="rId3"/>
     <sheet name="Meritalk" sheetId="4" r:id="rId4"/>
     <sheet name="AFCEA" sheetId="5" r:id="rId5"/>
+    <sheet name="AFFIRM" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="270" uniqueCount="231">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="290" uniqueCount="247">
   <si>
     <t>Event Name</t>
   </si>
@@ -715,6 +716,54 @@
   </si>
   <si>
     <t>https://afceadc.swoogo.com/milit23/</t>
+  </si>
+  <si>
+    <t>Virtual Monthly Speaker Series: Supply Chain Risk Management in a Global World</t>
+  </si>
+  <si>
+    <t>2023 Federal IT Career Workshop</t>
+  </si>
+  <si>
+    <t>Virtual Monthly Speaker Series: Building Blocks of Government in the Metaverse</t>
+  </si>
+  <si>
+    <t>Virtual Monthly Speaker Series: Emerging Technologies and AI</t>
+  </si>
+  <si>
+    <t>WedApril19</t>
+  </si>
+  <si>
+    <t>TueApril25</t>
+  </si>
+  <si>
+    <t>WedMay17</t>
+  </si>
+  <si>
+    <t>WedJune21</t>
+  </si>
+  <si>
+    <t>Thought leaders from government and industry discuss the nature of complex software environments and methods to better manage and mitigate supply chain risks.</t>
+  </si>
+  <si>
+    <t>Join AFFIRM for this in-person workshop as you navigate your path through a career in government.</t>
+  </si>
+  <si>
+    <t>Our panel will discuss the pitfalls and the promise of the future of technology in the metaverse.</t>
+  </si>
+  <si>
+    <t>Save the Date - event information coming soon!</t>
+  </si>
+  <si>
+    <t>https://associationforfederalinformationresourcesmanagementaffirm.growthzoneapp.com/ap/Events/Register/9p8B3mdL?sourceTypeId=Website&amp;mode=Attendee</t>
+  </si>
+  <si>
+    <t>https://associationforfederalinformationresourcesmanagementaffirm.growthzoneapp.com/ap/Events/Register/MrD67RZP?sourceTypeId=Website&amp;mode=Attendee</t>
+  </si>
+  <si>
+    <t>https://associationforfederalinformationresourcesmanagementaffirm.growthzoneapp.com/ap/Events/Register/Zrnd7e0P?sourceTypeId=Website&amp;mode=Attendee</t>
+  </si>
+  <si>
+    <t>https://associationforfederalinformationresourcesmanagementaffirm.growthzoneapp.com/ap/Events/Register/DpBbzVkp?sourceTypeId=Website&amp;mode=Attendee</t>
   </si>
 </sst>
 </file>
@@ -2163,4 +2212,93 @@
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:D5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:4">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2" t="s">
+        <v>231</v>
+      </c>
+      <c r="B2" t="s">
+        <v>235</v>
+      </c>
+      <c r="C2" t="s">
+        <v>239</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3" t="s">
+        <v>232</v>
+      </c>
+      <c r="B3" t="s">
+        <v>236</v>
+      </c>
+      <c r="C3" t="s">
+        <v>240</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="A4" t="s">
+        <v>233</v>
+      </c>
+      <c r="B4" t="s">
+        <v>237</v>
+      </c>
+      <c r="C4" t="s">
+        <v>241</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
+      <c r="A5" t="s">
+        <v>234</v>
+      </c>
+      <c r="B5" t="s">
+        <v>238</v>
+      </c>
+      <c r="C5" t="s">
+        <v>242</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>246</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="D2" r:id="rId1"/>
+    <hyperlink ref="D3" r:id="rId2"/>
+    <hyperlink ref="D4" r:id="rId3"/>
+    <hyperlink ref="D5" r:id="rId4"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>